<commit_message>
spring-boot-common easyexcel temp param
</commit_message>
<xml_diff>
--- a/spring-boot-common/src/main/resources/templates/easy_excel_params_temp.xlsx
+++ b/spring-boot-common/src/main/resources/templates/easy_excel_params_temp.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23250" windowHeight="12855"/>
+    <workbookView windowWidth="27945" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,14 +96,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,7 +443,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -462,6 +455,32 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -574,152 +593,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -727,7 +746,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1047,13 +1087,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="3" width="19.625" customWidth="1"/>
   </cols>
@@ -1118,24 +1158,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="C8" s="6"/>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="C1:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>